<commit_message>
Add DdemoBlaze Project Folder
</commit_message>
<xml_diff>
--- a/DemoBlaze_Testing.xlsx
+++ b/DemoBlaze_Testing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shiva\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shiva\DemoBlaze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518705F1-3834-4900-A059-1E0329901B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38AD2289-EA11-418A-A54F-81FEEBCA07E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7310" yWindow="1150" windowWidth="11890" windowHeight="7280" firstSheet="3" activeTab="5" xr2:uid="{2C072E80-1794-4824-8844-34245C702E7E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="9" xr2:uid="{2C072E80-1794-4824-8844-34245C702E7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenarioes" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="539">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -1959,40 +1959,43 @@
 "Wrong password." </t>
   </si>
   <si>
-    <t>C:\Users\ADMIN\Pictures\Screenshots\Sign-Up.png</t>
-  </si>
-  <si>
-    <t>C:\Users\ADMIN\Pictures\Screenshots\Login.png</t>
-  </si>
-  <si>
-    <t>C:\Users\ADMIN\Pictures\Screenshots\LogoutwithBrowserbackbtn.png</t>
-  </si>
-  <si>
-    <t>C:\Users\ADMIN\Pictures\Screenshots\Unsuccessful Login Attempts.png</t>
-  </si>
-  <si>
     <t>C:\Users\ADMIN\Pictures\Screenshots\Contact.png</t>
   </si>
   <si>
     <t>The message textarea box in the Contact Form allows users to enter more characters than the specified limit (e.g., 100 characters) without displaying any validation errors. This can lead to issues with data handling and user experience.</t>
   </si>
   <si>
-    <t>C:\Users\ADMIN\Pictures\Screenshots\Contact Message limit.png</t>
-  </si>
-  <si>
-    <t>C:\Users\ADMIN\Pictures\Screenshots\Contact with Invalid Email.png</t>
-  </si>
-  <si>
-    <t>C:\Users\ADMIN\Pictures\Screenshots\cart in quantity and total price.png</t>
-  </si>
-  <si>
-    <t>C:\Users\ADMIN\Pictures\Screenshots\Remove Item from Cart.png</t>
-  </si>
-  <si>
-    <t>C:\Users\ADMIN\Pictures\Screenshots\Phones Category.png</t>
-  </si>
-  <si>
-    <t>C:\Users\ADMIN\Pictures\Screenshots\Laptop Category.png</t>
+    <t>DemoBlaze_V-1.1\screenshots\Sign-Up.png</t>
+  </si>
+  <si>
+    <t>DemoBlaze_V-1.1\screenshots\Login.png</t>
+  </si>
+  <si>
+    <t>DemoBlaze_V-1.1\screenshots\LogoutwithBrowserbackbtn.png</t>
+  </si>
+  <si>
+    <t>DemoBlaze_V-1.1\screenshots\Unsuccessful Login Attempts.png</t>
+  </si>
+  <si>
+    <t>DemoBlaze_V-1.1\screenshots\Contact.png</t>
+  </si>
+  <si>
+    <t>DemoBlaze_V-1.1\screenshots\Contact with Invalid Email.png</t>
+  </si>
+  <si>
+    <t>DemoBlaze_V-1.1\screenshots\Contact Message limit.png</t>
+  </si>
+  <si>
+    <t>DemoBlaze_V-1.1\screenshots\cart in quantity and total price.png</t>
+  </si>
+  <si>
+    <t>DemoBlaze_V-1.1\screenshots\Remove Item from Cart.png</t>
+  </si>
+  <si>
+    <t>DemoBlaze_V-1.1\screenshots\Phones Category.png</t>
+  </si>
+  <si>
+    <t>DemoBlaze_V-1.1\screenshots\Laptop Category.png</t>
   </si>
 </sst>
 </file>
@@ -2926,8 +2929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{127605D1-D170-4159-8798-DCC696350102}">
   <dimension ref="A2:N17"/>
   <sheetViews>
-    <sheetView topLeftCell="F5" zoomScale="67" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="H14" zoomScale="67" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3023,7 +3026,7 @@
         <v>500</v>
       </c>
       <c r="M3" s="25" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="N3" s="20" t="s">
         <v>446</v>
@@ -3061,7 +3064,7 @@
         <v>486</v>
       </c>
       <c r="M4" s="25" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="N4" s="20" t="s">
         <v>446</v>
@@ -3099,7 +3102,7 @@
         <v>500</v>
       </c>
       <c r="M5" s="25" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="N5" s="20" t="s">
         <v>446</v>
@@ -3139,7 +3142,7 @@
         <v>374</v>
       </c>
       <c r="M6" s="25" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="N6" s="20" t="s">
         <v>446</v>
@@ -3179,7 +3182,7 @@
         <v>525</v>
       </c>
       <c r="M7" s="25" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="N7" s="20" t="s">
         <v>446</v>
@@ -3217,7 +3220,7 @@
         <v>486</v>
       </c>
       <c r="M8" s="25" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="N8" s="20" t="s">
         <v>446</v>
@@ -3255,7 +3258,7 @@
         <v>397</v>
       </c>
       <c r="M9" s="25" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="N9" s="20" t="s">
         <v>446</v>
@@ -3293,7 +3296,7 @@
         <v>398</v>
       </c>
       <c r="M10" s="25" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="N10" s="20" t="s">
         <v>446</v>
@@ -3358,7 +3361,7 @@
         <v>471</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="I12" s="20" t="s">
         <v>164</v>
@@ -3373,7 +3376,7 @@
         <v>401</v>
       </c>
       <c r="M12" s="25" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="N12" s="20" t="s">
         <v>446</v>
@@ -3411,7 +3414,7 @@
         <v>407</v>
       </c>
       <c r="M13" s="25" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="N13" s="20" t="s">
         <v>446</v>
@@ -3449,7 +3452,7 @@
         <v>408</v>
       </c>
       <c r="M14" s="25" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="N14" s="20" t="s">
         <v>446</v>
@@ -3487,7 +3490,7 @@
         <v>409</v>
       </c>
       <c r="M15" s="25" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="N15" s="20" t="s">
         <v>446</v>
@@ -3527,7 +3530,7 @@
         <v>418</v>
       </c>
       <c r="M16" s="25" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="N16" s="20" t="s">
         <v>446</v>
@@ -3567,7 +3570,7 @@
         <v>424</v>
       </c>
       <c r="M17" s="25" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="N17" s="20" t="s">
         <v>446</v>
@@ -3575,21 +3578,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M3" r:id="rId1" xr:uid="{9D3B0138-66DA-4727-A9F6-BA9AB5BC6092}"/>
-    <hyperlink ref="M4" r:id="rId2" xr:uid="{0362711C-DD9D-4496-B6E6-0B89D61D5278}"/>
-    <hyperlink ref="M5" r:id="rId3" xr:uid="{F629DF51-F1CA-4CE2-B515-28A621F726CB}"/>
-    <hyperlink ref="M6" r:id="rId4" xr:uid="{3EB97364-5E40-40B2-A1C4-2D61F8A8F4A0}"/>
-    <hyperlink ref="M7" r:id="rId5" xr:uid="{05CAB7F7-6A19-43E4-B6F6-304B7D3120B0}"/>
-    <hyperlink ref="M8" r:id="rId6" xr:uid="{E4CD43B1-4CD0-45E3-B815-8428DA7206A1}"/>
-    <hyperlink ref="M9" r:id="rId7" xr:uid="{AFB993D6-2968-48B4-AFB0-7B58C46C10D3}"/>
-    <hyperlink ref="M10" r:id="rId8" xr:uid="{C11A44EC-BBA0-4B1E-A97D-72F25134077C}"/>
-    <hyperlink ref="M12" r:id="rId9" xr:uid="{70B936D5-3C5A-43A6-BE54-700053F9E8F0}"/>
-    <hyperlink ref="M11" r:id="rId10" xr:uid="{AC30538B-5E5C-42D0-94C8-A8641A1A3787}"/>
-    <hyperlink ref="M13" r:id="rId11" xr:uid="{1E52D234-813B-40D7-80E0-EF767948B52D}"/>
-    <hyperlink ref="M15" r:id="rId12" xr:uid="{FAD013C7-E8E7-4CDD-98DE-07EFF6587920}"/>
-    <hyperlink ref="M14" r:id="rId13" xr:uid="{44691429-BA4E-4A6E-8933-2911C90ABEC7}"/>
-    <hyperlink ref="M16" r:id="rId14" xr:uid="{8E429EC5-95EA-494B-AF5F-7D483A037E14}"/>
-    <hyperlink ref="M17" r:id="rId15" xr:uid="{7E38DD00-B8BD-4A80-B703-F3C75D4501FC}"/>
+    <hyperlink ref="M10" r:id="rId1" xr:uid="{C11A44EC-BBA0-4B1E-A97D-72F25134077C}"/>
+    <hyperlink ref="M3" r:id="rId2" xr:uid="{578997E1-066A-4450-A139-334E16E73E44}"/>
+    <hyperlink ref="M4" r:id="rId3" xr:uid="{0DBDB39E-EBE1-44C5-A175-FB12272276E3}"/>
+    <hyperlink ref="M5" r:id="rId4" xr:uid="{CA9EEC70-DCE1-4967-96B7-B6384EDF08F3}"/>
+    <hyperlink ref="M6" r:id="rId5" xr:uid="{7A28D8CD-313D-45F2-91D1-7BE45C99FA39}"/>
+    <hyperlink ref="M7" r:id="rId6" xr:uid="{22AA1FAD-EF12-4B2A-A278-8B819A60CAAF}"/>
+    <hyperlink ref="M8" r:id="rId7" xr:uid="{78F0816E-AA9B-4496-A6AE-1A0BBFE35570}"/>
+    <hyperlink ref="M9" r:id="rId8" xr:uid="{8193509A-0572-456C-B987-6A98D1F4674C}"/>
+    <hyperlink ref="M11" r:id="rId9" xr:uid="{CC63F6B8-F956-40B7-B700-F0E2F67737B9}"/>
+    <hyperlink ref="M12" r:id="rId10" xr:uid="{AC74AB69-41FB-4FB6-AE22-0E1EE2CEA700}"/>
+    <hyperlink ref="M13" r:id="rId11" xr:uid="{C3DB48A8-1F8E-4CCC-84C1-C8F2EFCF927F}"/>
+    <hyperlink ref="M14" r:id="rId12" xr:uid="{13EE8EF8-797B-4C61-84DD-5E13F777AD21}"/>
+    <hyperlink ref="M15" r:id="rId13" xr:uid="{1073E8BB-E6BC-4862-8C96-B777D98371D3}"/>
+    <hyperlink ref="M16" r:id="rId14" xr:uid="{D35FE66A-15AF-4610-90BC-083DD410EE42}"/>
+    <hyperlink ref="M17" r:id="rId15" xr:uid="{2F028D39-C270-4B7C-870F-AD38F7C9714E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5111,7 +5114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C1288A-4D02-4533-A47C-4D93D2668B5C}">
   <dimension ref="A2:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="32" workbookViewId="0">
+    <sheetView topLeftCell="B3" zoomScale="32" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -5242,7 +5245,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="378" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="357" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>308</v>
       </c>

</xml_diff>